<commit_message>
OpenPyXL: Master Detail CSV: With Field Metadata
</commit_message>
<xml_diff>
--- a/python/openpyxl/csv-md/sample.xlsx
+++ b/python/openpyxl/csv-md/sample.xlsx
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="AB7" s="5" t="n">
-        <v>43843</v>
+        <v>43845</v>
       </c>
     </row>
     <row r="8">
@@ -919,7 +919,7 @@
         </is>
       </c>
       <c r="AB10" s="5" t="n">
-        <v>43844</v>
+        <v>43847</v>
       </c>
     </row>
     <row r="11">
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="AB13" s="5" t="n">
-        <v>43845</v>
+        <v>43848</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
LibreOffice Macro: Master Detail CSV: With Field Metadata
</commit_message>
<xml_diff>
--- a/python/openpyxl/csv-md/sample.xlsx
+++ b/python/openpyxl/csv-md/sample.xlsx
@@ -810,9 +810,7 @@
       <c r="AK8" s="7" t="n">
         <v>12000000</v>
       </c>
-      <c r="AL8" s="7" t="n">
-        <v>1200000</v>
-      </c>
+      <c r="AL8" s="7" t="n"/>
       <c r="AM8" s="2" t="n">
         <v>0</v>
       </c>
@@ -949,9 +947,7 @@
       <c r="AK11" s="7" t="n">
         <v>13000000</v>
       </c>
-      <c r="AL11" s="7" t="n">
-        <v>1300000</v>
-      </c>
+      <c r="AL11" s="7" t="n"/>
       <c r="AM11" s="2" t="n">
         <v>0</v>
       </c>
@@ -1088,9 +1084,7 @@
       <c r="AK14" s="7" t="n">
         <v>26000000</v>
       </c>
-      <c r="AL14" s="7" t="n">
-        <v>2600000</v>
-      </c>
+      <c r="AL14" s="7" t="n"/>
       <c r="AM14" s="2" t="n">
         <v>0</v>
       </c>
@@ -1114,20 +1108,18 @@
         <v>15000</v>
       </c>
       <c r="AH15" s="2" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="AI15" s="7" t="n">
-        <v>3000000</v>
+        <v>300000</v>
       </c>
       <c r="AJ15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AK15" s="7" t="n">
-        <v>3000000</v>
-      </c>
-      <c r="AL15" s="7" t="n">
         <v>300000</v>
       </c>
+      <c r="AL15" s="7" t="n"/>
       <c r="AM15" s="2" t="n">
         <v>0</v>
       </c>
@@ -1151,20 +1143,18 @@
         <v>8000</v>
       </c>
       <c r="AH16" s="2" t="n">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="AI16" s="7" t="n">
-        <v>40000000</v>
+        <v>4000000</v>
       </c>
       <c r="AJ16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AK16" s="7" t="n">
-        <v>40000000</v>
-      </c>
-      <c r="AL16" s="7" t="n">
         <v>4000000</v>
       </c>
+      <c r="AL16" s="7" t="n"/>
       <c r="AM16" s="2" t="n">
         <v>0</v>
       </c>

</xml_diff>